<commit_message>
13.12.2020 M C Sale s Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Retailer's payment format (Changed bkash no) of Rajshahi zone.xlsx
+++ b/2020/Others/Adding New Retailer Format/Retailer's payment format (Changed bkash no) of Rajshahi zone.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Dealer Name</t>
   </si>
@@ -40,43 +40,13 @@
     <t>Retail Name</t>
   </si>
   <si>
-    <t>RET-19352</t>
-  </si>
-  <si>
-    <t>Five Brothers</t>
-  </si>
-  <si>
-    <t>RET-35280</t>
-  </si>
-  <si>
-    <t>Sohan Electric &amp; Hardware</t>
-  </si>
-  <si>
-    <t>RET-36165</t>
-  </si>
-  <si>
-    <t>Azim Mobile Center</t>
-  </si>
-  <si>
-    <t>RET-36167</t>
-  </si>
-  <si>
-    <t>Gourango Hardware</t>
-  </si>
-  <si>
-    <t>Bishakhi Enterprise</t>
-  </si>
-  <si>
-    <t>RET-34130</t>
-  </si>
-  <si>
-    <t>CD Sound &amp; Electronics</t>
-  </si>
-  <si>
-    <t>RET-34136</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>RET-26511</t>
+  </si>
+  <si>
+    <t>Bismillah Telecom</t>
   </si>
 </sst>
 </file>
@@ -141,11 +111,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +427,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -485,112 +461,61 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3">
-        <v>1746161400</v>
+      <c r="F2" s="5">
+        <v>1316416301</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1860207883</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1764994148</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1722309632</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1718898690</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1730430130</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2"/>
@@ -632,7 +557,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>